<commit_message>
Adaptação estratégia e refatoração
</commit_message>
<xml_diff>
--- a/extracteds/Cases/Compra fechamento e venda com 0.80% (Exceto Sexta).xlsx
+++ b/extracteds/Cases/Compra fechamento e venda com 0.80% (Exceto Sexta).xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>Ativo</t>
   </si>
@@ -57,13 +57,16 @@
     <t xml:space="preserve">Volume Med</t>
   </si>
   <si>
-    <t>BLUT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-24 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-27 10:05:00</t>
+    <t>Stop_loss</t>
+  </si>
+  <si>
+    <t>CASH3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12-17 10:10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-28 10:10:00</t>
   </si>
   <si>
     <r>
@@ -95,368 +98,194 @@
       <t xml:space="preserve"> com 0.80% de gain(Vender no leilão de abertura poderá potencializar os lucros).
 Se o stop-gain não for atingido, vender no fechamento!
 Período de teste: 15/12/2021 a 20/06/2022
-Alterar: caseCompraFechamentoNegativo.py</t>
+Alterar: caseCompraFechamentoNegativo(StopLoss).py</t>
     </r>
   </si>
   <si>
+    <t>CIEL3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-24 10:05:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-18 10:05:00</t>
+  </si>
+  <si>
+    <t>COGN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-25 10:05:00</t>
+  </si>
+  <si>
+    <t>DMMO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-01 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-17 10:10:00</t>
+  </si>
+  <si>
+    <t>ELET6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-07 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-12 10:05:00</t>
+  </si>
+  <si>
+    <t>ENAT3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12-17 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-17 10:00:00</t>
+  </si>
+  <si>
+    <t>GFSA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-05 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-04-12 11:00:00</t>
+  </si>
+  <si>
+    <t>MYPK3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-14 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-10 10:05:00</t>
+  </si>
+  <si>
+    <t>NEXP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-24 10:10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-02 10:05:00</t>
+  </si>
+  <si>
+    <t>NUBR33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-03 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-17 10:15:00</t>
+  </si>
+  <si>
+    <t>PETR3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-24 10:05:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-10 10:05:00</t>
+  </si>
+  <si>
+    <t>PETR4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-06 10:05:00</t>
+  </si>
+  <si>
+    <t>PRIO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-05 10:10:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-10 10:10:00</t>
+  </si>
+  <si>
+    <t>RECV3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2021-12-17 10:05:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-04 10:05:00</t>
+  </si>
+  <si>
+    <t>RRRP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-05 10:05:00</t>
+  </si>
+  <si>
+    <t>SLCE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-05-12 10:05:00</t>
+  </si>
+  <si>
+    <t>SYNE3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-25 10:10:00</t>
+  </si>
+  <si>
+    <t>TCSA3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-24 10:00:00</t>
+  </si>
+  <si>
+    <t>TECN3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-02-09 10:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-30 10:10:00</t>
+  </si>
+  <si>
     <t>TRAD3</t>
   </si>
   <si>
     <t xml:space="preserve">2022-01-03 10:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-02-25 10:10:00</t>
-  </si>
-  <si>
-    <t>DMMO3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-06 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-17 10:10:00</t>
+    <t>VIIA3</t>
   </si>
   <si>
     <t>VIVR3</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-03-31 10:05:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">2022-03-29 10:10:00</t>
   </si>
   <si>
+    <t>WEST3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-20 10:10:00</t>
+  </si>
+  <si>
+    <t>INEP3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-01-26 10:20:00</t>
+  </si>
+  <si>
     <t>LUPA3</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-12-17 10:00:00</t>
+    <t xml:space="preserve">2022-01-11 10:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">2022-03-08 10:05:00</t>
   </si>
   <si>
-    <t>NEXP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-11 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-02 10:05:00</t>
-  </si>
-  <si>
-    <t>WEST3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-03 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-20 10:10:00</t>
-  </si>
-  <si>
-    <t>TCSA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-05 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-01 10:00:00</t>
-  </si>
-  <si>
-    <t>TECN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-09 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-30 10:10:00</t>
-  </si>
-  <si>
-    <t>COGN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-20 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-25 10:05:00</t>
-  </si>
-  <si>
     <t>OIBR3</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-06-10 10:10:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">2022-01-28 10:20:00</t>
-  </si>
-  <si>
-    <t>BRIT3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-06 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-04 10:05:00</t>
-  </si>
-  <si>
-    <t>GFSA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-05 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-12 11:00:00</t>
-  </si>
-  <si>
-    <t>PRIO3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-05 10:10:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-10 10:10:00</t>
-  </si>
-  <si>
-    <t>DASA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-03 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-04 10:05:00</t>
-  </si>
-  <si>
-    <t>NTCO3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-06 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-10 10:05:00</t>
-  </si>
-  <si>
-    <t>ENJU3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-25 10:10:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-11 10:10:00</t>
-  </si>
-  <si>
-    <t>NGRD3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-16 10:10:00</t>
-  </si>
-  <si>
-    <t>FHER3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-05 10:10:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-17 10:15:00</t>
-  </si>
-  <si>
-    <t>MGLU3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-12 10:05:00</t>
-  </si>
-  <si>
-    <t>SLCE3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-15 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-12 10:05:00</t>
-  </si>
-  <si>
-    <t>CSED3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-10 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-27 10:05:00</t>
-  </si>
-  <si>
-    <t>NUBR33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-17 10:15:00</t>
-  </si>
-  <si>
-    <t>PLPL3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-11 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-01 10:10:00</t>
-  </si>
-  <si>
-    <t>VIIA3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-08 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-10 10:05:00</t>
-  </si>
-  <si>
-    <t>CASH3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-06 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-28 10:10:00</t>
-  </si>
-  <si>
-    <t>RECV3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-04 10:05:00</t>
-  </si>
-  <si>
-    <t>MYPK3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-04 10:00:00</t>
-  </si>
-  <si>
-    <t>PETR4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-27 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-06 10:05:00</t>
-  </si>
-  <si>
-    <t>PETR3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-17 10:15:00</t>
-  </si>
-  <si>
-    <t>RRRP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-23 10:05:00</t>
-  </si>
-  <si>
-    <t>CIEL3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-18 10:05:00</t>
-  </si>
-  <si>
-    <t>ENEV3</t>
-  </si>
-  <si>
-    <t>CVCB3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-06 10:10:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-16 10:20:00</t>
-  </si>
-  <si>
-    <t>ELET6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-10 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-12 10:05:00</t>
-  </si>
-  <si>
-    <t>GETT11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-21 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-20 10:15:00</t>
-  </si>
-  <si>
-    <t>VULC3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-07 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-31 10:00:00</t>
-  </si>
-  <si>
-    <t>LREN3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-26 10:10:00</t>
-  </si>
-  <si>
-    <t>LAVV3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-12 10:00:00</t>
-  </si>
-  <si>
-    <t>SYNE3</t>
-  </si>
-  <si>
-    <t>HYPE3</t>
-  </si>
-  <si>
-    <t>RANI3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-08 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-29 10:05:00</t>
-  </si>
-  <si>
-    <t>RAPT4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-26 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-04 10:00:00</t>
-  </si>
-  <si>
-    <t>BMGB4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-21 10:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-03-09 10:00:00</t>
-  </si>
-  <si>
-    <t>JSLG3</t>
-  </si>
-  <si>
-    <t>BRML3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-05-18 10:10:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-04-19 10:05:00</t>
-  </si>
-  <si>
-    <t>INEP3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-06-14 10:05:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-01-26 10:20:00</t>
   </si>
 </sst>
 </file>
@@ -997,52 +826,58 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2">
         <v>102</v>
       </c>
       <c r="D2" s="2">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F2" s="3">
-        <v>0.9509803921568627</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="G2" s="3">
-        <v>1.429066666615453</v>
+        <v>0.39008986028625831</v>
       </c>
       <c r="H2" s="3">
-        <v>1.4010457515837774e-002</v>
+        <v>3.8244103949633167e-003</v>
       </c>
       <c r="I2" s="3">
-        <v>-8.8235294117647078e-002</v>
+        <v>-6.6166666666666651e-002</v>
       </c>
       <c r="J2" s="3">
-        <v>0.1153846153846152</v>
+        <v>4.4067796610169463e-002</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" s="2">
-        <v>136600</v>
+        <v>7454500</v>
       </c>
       <c r="N2" s="2">
-        <v>654255.5555555555</v>
+        <v>38302714.173228346</v>
+      </c>
+      <c r="O2" s="3">
+        <v>-6.6166666666666651e-002</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
@@ -1057,46 +892,49 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C3" s="2">
         <v>102</v>
       </c>
       <c r="D3" s="2">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E3" s="2">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3">
-        <v>0.93137254901960786</v>
+        <v>0.80392156862745101</v>
       </c>
       <c r="G3" s="3">
-        <v>0.60838437231140352</v>
+        <v>0.37175590875431902</v>
       </c>
       <c r="H3" s="3">
-        <v>5.9645526697196423e-003</v>
+        <v>3.6446657721011669e-003</v>
       </c>
       <c r="I3" s="3">
-        <v>-8.1939799331103735e-002</v>
+        <v>-5.7639534883720922e-002</v>
       </c>
       <c r="J3" s="3">
-        <v>3.5046728971962482e-002</v>
+        <v>6.800000000000006e-002</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M3" s="2">
-        <v>907700</v>
+        <v>4614900</v>
       </c>
       <c r="N3" s="2">
-        <v>2567502.3809523811</v>
+        <v>32772901.574803151</v>
+      </c>
+      <c r="O3" s="3">
+        <v>-5.7639534883720922e-002</v>
       </c>
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
@@ -1112,46 +950,49 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C4" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4" s="2">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E4" s="2">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3">
-        <v>0.93000000000000005</v>
+        <v>0.87254901960784315</v>
       </c>
       <c r="G4" s="3">
-        <v>0.78969298072600813</v>
+        <v>0.53111673343399157</v>
       </c>
       <c r="H4" s="3">
-        <v>7.8969298072600821e-003</v>
+        <v>5.2070267983724662e-003</v>
       </c>
       <c r="I4" s="3">
-        <v>-0.11176470588235288</v>
+        <v>-8.3533613445378074e-002</v>
       </c>
       <c r="J4" s="3">
-        <v>5.9829059829059839e-002</v>
+        <v>5.6277056277056259e-002</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>23</v>
       </c>
       <c r="M4" s="2">
-        <v>1013600</v>
+        <v>7426200</v>
       </c>
       <c r="N4" s="2">
-        <v>20533882.258064516</v>
+        <v>34852972.44094488</v>
+      </c>
+      <c r="O4" s="3">
+        <v>-8.3533613445378074e-002</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
@@ -1170,31 +1011,31 @@
         <v>24</v>
       </c>
       <c r="B5" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C5" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D5" s="2">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="3">
-        <v>0.91000000000000003</v>
+        <v>0.92156862745098034</v>
       </c>
       <c r="G5" s="3">
-        <v>0.63169361377089883</v>
+        <v>0.72309829428190242</v>
       </c>
       <c r="H5" s="3">
-        <v>6.3169361377089887e-003</v>
+        <v>7.0891989635480631e-003</v>
       </c>
       <c r="I5" s="3">
-        <v>-8.3969465648854991e-002</v>
+        <v>-7.7625000000000111e-002</v>
       </c>
       <c r="J5" s="3">
-        <v>3.007518796992481e-002</v>
+        <v>5.9829059829059839e-002</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>25</v>
@@ -1203,10 +1044,13 @@
         <v>26</v>
       </c>
       <c r="M5" s="2">
-        <v>1159800</v>
+        <v>1013600</v>
       </c>
       <c r="N5" s="2">
-        <v>4007595.1612903224</v>
+        <v>20354196.062992126</v>
+      </c>
+      <c r="O5" s="3">
+        <v>-7.7625000000000111e-002</v>
       </c>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
@@ -1225,31 +1069,31 @@
         <v>27</v>
       </c>
       <c r="B6" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C6" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D6" s="2">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E6" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F6" s="3">
-        <v>0.90000000000000002</v>
+        <v>0.80392156862745101</v>
       </c>
       <c r="G6" s="3">
-        <v>0.51057018524557574</v>
+        <v>0.38750724060676345</v>
       </c>
       <c r="H6" s="3">
-        <v>5.1057018524557577e-003</v>
+        <v>3.7990905941839553e-003</v>
       </c>
       <c r="I6" s="3">
-        <v>-5.5932203389830515e-002</v>
+        <v>-3.6786380113930595e-002</v>
       </c>
       <c r="J6" s="3">
-        <v>3.3755274261603407e-002</v>
+        <v>3.47947112038971e-002</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>28</v>
@@ -1258,10 +1102,13 @@
         <v>29</v>
       </c>
       <c r="M6" s="2">
-        <v>236800</v>
+        <v>741300</v>
       </c>
       <c r="N6" s="2">
-        <v>1137571.7741935484</v>
+        <v>3606908.6614173227</v>
+      </c>
+      <c r="O6" s="3">
+        <v>-3.6786380113930595e-002</v>
       </c>
       <c r="P6" s="5"/>
       <c r="Q6" s="5"/>
@@ -1280,31 +1127,31 @@
         <v>30</v>
       </c>
       <c r="B7" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C7" s="2">
         <v>102</v>
       </c>
       <c r="D7" s="2">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E7" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3">
-        <v>0.89215686274509809</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="G7" s="3">
-        <v>0.77262700985913035</v>
+        <v>0.3237959677572757</v>
       </c>
       <c r="H7" s="3">
-        <v>7.5747746064620623e-003</v>
+        <v>3.1744702721301539e-003</v>
       </c>
       <c r="I7" s="3">
-        <v>-6.1403508771929904e-002</v>
+        <v>-3.396528129751647e-002</v>
       </c>
       <c r="J7" s="3">
-        <v>6.5040650406504197e-002</v>
+        <v>2.6740665993945534e-002</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>31</v>
@@ -1313,10 +1160,13 @@
         <v>32</v>
       </c>
       <c r="M7" s="2">
-        <v>229300</v>
+        <v>544200</v>
       </c>
       <c r="N7" s="2">
-        <v>1264538.888888889</v>
+        <v>2115507.874015748</v>
+      </c>
+      <c r="O7" s="3">
+        <v>-3.396528129751647e-002</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
@@ -1335,31 +1185,31 @@
         <v>33</v>
       </c>
       <c r="B8" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C8" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E8" s="2">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F8" s="3">
-        <v>0.89215686274509809</v>
+        <v>0.85999999999999999</v>
       </c>
       <c r="G8" s="3">
-        <v>0.67291255913556913</v>
+        <v>0.33156340563166214</v>
       </c>
       <c r="H8" s="3">
-        <v>6.5971819523095009e-003</v>
+        <v>3.3156340563166215e-003</v>
       </c>
       <c r="I8" s="3">
-        <v>-6.719367588932823e-002</v>
+        <v>-7.5586956521739135e-002</v>
       </c>
       <c r="J8" s="3">
-        <v>3.114186851211076e-002</v>
+        <v>3.7433155080213831e-002</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>34</v>
@@ -1368,10 +1218,13 @@
         <v>35</v>
       </c>
       <c r="M8" s="2">
-        <v>193500</v>
+        <v>2464100</v>
       </c>
       <c r="N8" s="2">
-        <v>868307.14285714284</v>
+        <v>6698545.1612903224</v>
+      </c>
+      <c r="O8" s="3">
+        <v>-7.5586956521739135e-002</v>
       </c>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -1390,31 +1243,31 @@
         <v>36</v>
       </c>
       <c r="B9" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C9" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D9" s="2">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E9" s="2">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3">
-        <v>0.89000000000000001</v>
+        <v>0.81372549019607843</v>
       </c>
       <c r="G9" s="3">
-        <v>0.37642240148513867</v>
+        <v>0.35312816080581</v>
       </c>
       <c r="H9" s="3">
-        <v>3.7642240148513867e-003</v>
+        <v>3.4620407922138236e-003</v>
       </c>
       <c r="I9" s="3">
-        <v>-7.5907590759075938e-002</v>
+        <v>-2.8271929824561448e-002</v>
       </c>
       <c r="J9" s="3">
-        <v>2.4930747922437657e-002</v>
+        <v>4.146730462519943e-002</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>37</v>
@@ -1423,10 +1276,13 @@
         <v>38</v>
       </c>
       <c r="M9" s="2">
-        <v>192300</v>
+        <v>232000</v>
       </c>
       <c r="N9" s="2">
-        <v>609450.80645161285</v>
+        <v>1550493.7007874015</v>
+      </c>
+      <c r="O9" s="3">
+        <v>-2.8271929824561448e-002</v>
       </c>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
@@ -1445,31 +1301,31 @@
         <v>39</v>
       </c>
       <c r="B10" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D10" s="2">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E10" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" s="3">
-        <v>0.89000000000000001</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G10" s="3">
-        <v>0.53925734944818249</v>
+        <v>0.71507690778695565</v>
       </c>
       <c r="H10" s="3">
-        <v>5.3925734944818247e-003</v>
+        <v>7.0105579194799572e-003</v>
       </c>
       <c r="I10" s="3">
-        <v>-8.273381294964044e-002</v>
+        <v>-5.0000000000000044e-002</v>
       </c>
       <c r="J10" s="3">
-        <v>3.2051282051282159e-002</v>
+        <v>6.5040650406504197e-002</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>40</v>
@@ -1478,10 +1334,13 @@
         <v>41</v>
       </c>
       <c r="M10" s="2">
-        <v>210600</v>
+        <v>229300</v>
       </c>
       <c r="N10" s="2">
-        <v>1142588.7096774194</v>
+        <v>1256992.125984252</v>
+      </c>
+      <c r="O10" s="3">
+        <v>-3.7595238095238181e-002</v>
       </c>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
@@ -1500,31 +1359,31 @@
         <v>42</v>
       </c>
       <c r="B11" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D11" s="2">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E11" s="2">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F11" s="3">
-        <v>0.88</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G11" s="3">
-        <v>0.61612433972854186</v>
+        <v>0.41601398050641003</v>
       </c>
       <c r="H11" s="3">
-        <v>6.1612433972854184e-003</v>
+        <v>4.0785684363373528e-003</v>
       </c>
       <c r="I11" s="3">
-        <v>-7.3170731707317027e-002</v>
+        <v>-0.10785913312693501</v>
       </c>
       <c r="J11" s="3">
-        <v>5.6277056277056259e-002</v>
+        <v>0.10684931506849327</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>43</v>
@@ -1533,10 +1392,13 @@
         <v>44</v>
       </c>
       <c r="M11" s="2">
-        <v>11684000</v>
+        <v>696225</v>
       </c>
       <c r="N11" s="2">
-        <v>35036931.451612905</v>
+        <v>6642299.9055118114</v>
+      </c>
+      <c r="O11" s="3">
+        <v>-0.10785913312693501</v>
       </c>
       <c r="P11" s="5"/>
       <c r="Q11" s="5"/>
@@ -1555,31 +1417,31 @@
         <v>45</v>
       </c>
       <c r="B12" s="2">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C12" s="2">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D12" s="2">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E12" s="2">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3">
-        <v>0.88</v>
+        <v>0.82075471698113212</v>
       </c>
       <c r="G12" s="3">
-        <v>0.59313822894065538</v>
+        <v>0.41434957547359719</v>
       </c>
       <c r="H12" s="3">
-        <v>5.9313822894065541e-003</v>
+        <v>3.908958259184879e-003</v>
       </c>
       <c r="I12" s="3">
-        <v>-8.3333333333333259e-002</v>
+        <v>-3.9819260096017994e-002</v>
       </c>
       <c r="J12" s="3">
-        <v>5.9405940594059459e-002</v>
+        <v>4.3463263194204904e-002</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>46</v>
@@ -1588,10 +1450,13 @@
         <v>47</v>
       </c>
       <c r="M12" s="2">
-        <v>24885500</v>
+        <v>6224000</v>
       </c>
       <c r="N12" s="2">
-        <v>81054071.774193555</v>
+        <v>18183554.580152672</v>
+      </c>
+      <c r="O12" s="3">
+        <v>-2.728707733511887e-002</v>
       </c>
     </row>
     <row r="13">
@@ -1599,1584 +1464,1032 @@
         <v>48</v>
       </c>
       <c r="B13" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C13" s="2">
         <v>102</v>
       </c>
       <c r="D13" s="2">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E13" s="2">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3">
-        <v>0.87254901960784315</v>
+        <v>0.81372549019607843</v>
       </c>
       <c r="G13" s="3">
-        <v>0.74405464579099612</v>
+        <v>0.40239276850603417</v>
       </c>
       <c r="H13" s="3">
-        <v>7.2946533901078053e-003</v>
+        <v>3.9450271422160213e-003</v>
       </c>
       <c r="I13" s="3">
-        <v>-8.2222222222222197e-002</v>
+        <v>-4.1474654377880116e-002</v>
       </c>
       <c r="J13" s="3">
-        <v>5.4919908466819267e-002</v>
+        <v>2.1195274496177863e-002</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="M13" s="2">
-        <v>188900</v>
+        <v>28713600</v>
       </c>
       <c r="N13" s="2">
-        <v>627026.19047619053</v>
+        <v>73272579.527559057</v>
+      </c>
+      <c r="O13" s="3">
+        <v>-3.2104925424904562e-002</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C14" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D14" s="2">
         <v>87</v>
       </c>
       <c r="E14" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F14" s="3">
-        <v>0.87</v>
+        <v>0.8529411764705882</v>
       </c>
       <c r="G14" s="3">
-        <v>0.41506164299946469</v>
+        <v>0.61113937113690064</v>
       </c>
       <c r="H14" s="3">
-        <v>4.1506164299946469e-003</v>
+        <v>5.9915624621264766e-003</v>
       </c>
       <c r="I14" s="3">
-        <v>-7.5675675675675791e-002</v>
+        <v>-5.5102716468590829e-002</v>
       </c>
       <c r="J14" s="3">
-        <v>3.7433155080213831e-002</v>
+        <v>3.5577658760520325e-002</v>
       </c>
       <c r="K14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="M14" s="2">
-        <v>2464100</v>
+        <v>9086300</v>
       </c>
       <c r="N14" s="2">
-        <v>6698545.1612903224</v>
+        <v>20583591.338582676</v>
+      </c>
+      <c r="O14" s="3">
+        <v>-5.5102716468590829e-002</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="2">
+        <v>127</v>
+      </c>
+      <c r="C15" s="2">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2">
+        <v>84</v>
+      </c>
+      <c r="E15" s="2">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.82352941176470584</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.34222315428824418</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3.3551289636102369e-003</v>
+      </c>
+      <c r="I15" s="3">
+        <v>-4.1348844472204938e-002</v>
+      </c>
+      <c r="J15" s="3">
+        <v>3.5322777101096214e-002</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="2">
-        <v>124</v>
-      </c>
-      <c r="C15" s="2">
-        <v>100</v>
-      </c>
-      <c r="D15" s="2">
-        <v>87</v>
-      </c>
-      <c r="E15" s="2">
-        <v>13</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.87</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0.66070231129949375</v>
-      </c>
-      <c r="H15" s="3">
-        <v>6.6070231129949373e-003</v>
-      </c>
-      <c r="I15" s="3">
-        <v>-0.10762548262548266</v>
-      </c>
-      <c r="J15" s="3">
-        <v>3.5577658760520325e-002</v>
-      </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="M15" s="2">
-        <v>9086300</v>
+        <v>219600</v>
       </c>
       <c r="N15" s="2">
-        <v>20540425</v>
+        <v>1080868.5039370079</v>
+      </c>
+      <c r="O15" s="3">
+        <v>-4.1348844472204938e-002</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2">
+        <v>127</v>
+      </c>
+      <c r="C16" s="2">
+        <v>102</v>
+      </c>
+      <c r="D16" s="2">
+        <v>83</v>
+      </c>
+      <c r="E16" s="2">
+        <v>19</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.81372549019607843</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.44126980568686808</v>
+      </c>
+      <c r="H16" s="3">
+        <v>4.32617456555753e-003</v>
+      </c>
+      <c r="I16" s="3">
+        <v>-5.0540775591673748e-002</v>
+      </c>
+      <c r="J16" s="3">
+        <v>4.4634377967711414e-002</v>
+      </c>
+      <c r="K16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="2">
-        <v>124</v>
-      </c>
-      <c r="C16" s="2">
-        <v>100</v>
-      </c>
-      <c r="D16" s="2">
-        <v>86</v>
-      </c>
-      <c r="E16" s="2">
-        <v>14</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.85999999999999999</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.53726087052417537</v>
-      </c>
-      <c r="H16" s="3">
-        <v>5.372608705241754e-003</v>
-      </c>
-      <c r="I16" s="3">
-        <v>-7.4327405380756884e-002</v>
-      </c>
-      <c r="J16" s="3">
-        <v>3.076923076923066e-002</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="L16" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
       <c r="M16" s="2">
-        <v>123600</v>
+        <v>760400</v>
       </c>
       <c r="N16" s="2">
-        <v>425038.70967741933</v>
+        <v>4209766.9291338585</v>
+      </c>
+      <c r="O16" s="3">
+        <v>-5.0540775591673748e-002</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C17" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D17" s="2">
         <v>86</v>
       </c>
       <c r="E17" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F17" s="3">
-        <v>0.85999999999999999</v>
+        <v>0.84313725490196079</v>
       </c>
       <c r="G17" s="3">
-        <v>0.41548660233057699</v>
+        <v>0.44079632813011149</v>
       </c>
       <c r="H17" s="3">
-        <v>4.1548660233057698e-003</v>
+        <v>4.3215326287265833e-003</v>
       </c>
       <c r="I17" s="3">
-        <v>-7.258938244853741e-002</v>
+        <v>-2.0613243761996192e-002</v>
       </c>
       <c r="J17" s="3">
-        <v>6.3811922753988171e-002</v>
+        <v>2.8000000000000025e-002</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M17" s="2">
-        <v>2382900</v>
+        <v>488700</v>
       </c>
       <c r="N17" s="2">
-        <v>12193283.064516129</v>
+        <v>1796082.6771653544</v>
+      </c>
+      <c r="O17" s="3">
+        <v>-2.0613243761996192e-002</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C18" s="2">
         <v>102</v>
       </c>
       <c r="D18" s="2">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E18" s="2">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F18" s="3">
-        <v>0.8529411764705882</v>
+        <v>0.77450980392156865</v>
       </c>
       <c r="G18" s="3">
-        <v>0.40470200609660761</v>
+        <v>0.37658247517523735</v>
       </c>
       <c r="H18" s="3">
-        <v>3.9676667264373295e-003</v>
+        <v>3.6919850507376212e-003</v>
       </c>
       <c r="I18" s="3">
-        <v>-8.3892617449664475e-002</v>
+        <v>-2.4009803921568651e-002</v>
       </c>
       <c r="J18" s="3">
-        <v>6.4102564102564319e-002</v>
+        <v>7.986111111111116e-002</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M18" s="2">
-        <v>779000</v>
+        <v>103300</v>
       </c>
       <c r="N18" s="2">
-        <v>2678733.3333333335</v>
+        <v>1161411.8110236221</v>
+      </c>
+      <c r="O18" s="3">
+        <v>-2.4009803921568651e-002</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C19" s="2">
         <v>102</v>
       </c>
       <c r="D19" s="2">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E19" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3">
-        <v>0.8529411764705882</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G19" s="3">
-        <v>0.35661428979597792</v>
+        <v>0.34387135848071898</v>
       </c>
       <c r="H19" s="3">
-        <v>3.4962185274115482e-003</v>
+        <v>3.3712878282423429e-003</v>
       </c>
       <c r="I19" s="3">
-        <v>-6.8592057761732828e-002</v>
+        <v>-6.2900576368875971e-002</v>
       </c>
       <c r="J19" s="3">
-        <v>4.2918454935622297e-002</v>
+        <v>2.4930747922437657e-002</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="M19" s="2">
-        <v>323200</v>
+        <v>123600</v>
       </c>
       <c r="N19" s="2">
-        <v>1398037.3015873015</v>
+        <v>601720.47244094487</v>
+      </c>
+      <c r="O19" s="3">
+        <v>-6.2900576368875971e-002</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B20" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C20" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D20" s="2">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E20" s="2">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20" s="3">
-        <v>0.84999999999999998</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G20" s="3">
-        <v>0.34608996619256327</v>
+        <v>0.47430913474805336</v>
       </c>
       <c r="H20" s="3">
-        <v>3.4608996619256327e-003</v>
+        <v>4.6500895563534646e-003</v>
       </c>
       <c r="I20" s="3">
-        <v>-0.10537634408602159</v>
+        <v>-7.7841013824884786e-002</v>
       </c>
       <c r="J20" s="3">
-        <v>8.3276912660798841e-002</v>
+        <v>3.2051282051282159e-002</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M20" s="2">
-        <v>187100</v>
+        <v>151400</v>
       </c>
       <c r="N20" s="2">
-        <v>1112011.2903225806</v>
+        <v>1127767.716535433</v>
+      </c>
+      <c r="O20" s="3">
+        <v>-7.7841013824884786e-002</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B21" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C21" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D21" s="2">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E21" s="2">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F21" s="3">
-        <v>0.84999999999999998</v>
+        <v>0.92156862745098034</v>
       </c>
       <c r="G21" s="3">
-        <v>0.32978839133412868</v>
+        <v>0.5606502734640203</v>
       </c>
       <c r="H21" s="3">
-        <v>3.2978839133412869e-003</v>
+        <v>5.4965713084707876e-003</v>
       </c>
       <c r="I21" s="3">
-        <v>-0.10707070707070709</v>
+        <v>-6.2606796116504937e-002</v>
       </c>
       <c r="J21" s="3">
-        <v>3.9473684210526327e-002</v>
+        <v>3.5046728971962482e-002</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="M21" s="2">
-        <v>61801100</v>
+        <v>907700</v>
       </c>
       <c r="N21" s="2">
-        <v>130369149.19354838</v>
+        <v>2559045.6692913384</v>
+      </c>
+      <c r="O21" s="3">
+        <v>-6.2606796116504937e-002</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B22" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C22" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D22" s="2">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E22" s="2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F22" s="3">
-        <v>0.84999999999999998</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="G22" s="3">
-        <v>0.46706476038370753</v>
+        <v>0.35622807575407417</v>
       </c>
       <c r="H22" s="3">
-        <v>4.670647603837075e-003</v>
+        <v>3.4924321152360214e-003</v>
       </c>
       <c r="I22" s="3">
-        <v>-4.8104008667388953e-002</v>
+        <v>-7.8034031413612481e-002</v>
       </c>
       <c r="J22" s="3">
-        <v>2.8000000000000025e-002</v>
+        <v>4.8327137546468446e-002</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="M22" s="2">
-        <v>656400</v>
+        <v>19955500</v>
       </c>
       <c r="N22" s="2">
-        <v>1806935.4838709678</v>
+        <v>53162624.409448817</v>
+      </c>
+      <c r="O22" s="3">
+        <v>-7.8034031413612481e-002</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B23" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C23" s="2">
         <v>102</v>
       </c>
       <c r="D23" s="2">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E23" s="2">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F23" s="3">
-        <v>0.84313725490196079</v>
+        <v>0.89215686274509809</v>
       </c>
       <c r="G23" s="3">
-        <v>0.31331132708748871</v>
+        <v>0.67263130540160976</v>
       </c>
       <c r="H23" s="3">
-        <v>3.0716796773283205e-003</v>
+        <v>6.5944245627608802e-003</v>
       </c>
       <c r="I23" s="3">
-        <v>-7.7586206896551713e-002</v>
+        <v>-4.9019607843137303e-002</v>
       </c>
       <c r="J23" s="3">
-        <v>3.0874785591766596e-002</v>
+        <v>3.007518796992481e-002</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="M23" s="2">
-        <v>125700</v>
+        <v>1159800</v>
       </c>
       <c r="N23" s="2">
-        <v>679165.07936507941</v>
+        <v>3955071.653543307</v>
+      </c>
+      <c r="O23" s="3">
+        <v>-2.8626213592232996e-002</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C24" s="2">
         <v>102</v>
       </c>
       <c r="D24" s="2">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E24" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F24" s="3">
-        <v>0.84313725490196079</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G24" s="3">
-        <v>0.538941732926288</v>
+        <v>0.59597202547287931</v>
       </c>
       <c r="H24" s="3">
-        <v>5.28374247966949e-003</v>
+        <v>5.8428629948321497e-003</v>
       </c>
       <c r="I24" s="3">
-        <v>-0.10079051383399207</v>
+        <v>-6.7067567567567654e-002</v>
       </c>
       <c r="J24" s="3">
-        <v>0.10684931506849327</v>
+        <v>3.114186851211076e-002</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="M24" s="2">
-        <v>696225</v>
+        <v>109300</v>
       </c>
       <c r="N24" s="2">
-        <v>6683000</v>
+        <v>862330.70866141736</v>
+      </c>
+      <c r="O24" s="3">
+        <v>-6.7067567567567654e-002</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C25" s="2">
         <v>102</v>
       </c>
       <c r="D25" s="2">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E25" s="2">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="F25" s="3">
-        <v>0.84313725490196079</v>
+        <v>0.73529411764705888</v>
       </c>
       <c r="G25" s="3">
-        <v>0.53134804065630736</v>
+        <v>0.61647950966407361</v>
       </c>
       <c r="H25" s="3">
-        <v>5.2092945162383079e-003</v>
+        <v>6.0439167614124868e-003</v>
       </c>
       <c r="I25" s="3">
-        <v>-8.6206896551724088e-002</v>
+        <v>-5.2287581699346442e-002</v>
       </c>
       <c r="J25" s="3">
-        <v>3.4351145038167941e-002</v>
+        <v>0.33333333333333326</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="M25" s="2">
-        <v>255700</v>
+        <v>243700</v>
       </c>
       <c r="N25" s="2">
-        <v>793150</v>
+        <v>1208396.062992126</v>
+      </c>
+      <c r="O25" s="3">
+        <v>-3.7093984962406068e-002</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B26" s="2">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C26" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D26" s="2">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E26" s="2">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F26" s="3">
-        <v>0.83999999999999997</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="G26" s="3">
-        <v>0.46659198308134553</v>
+        <v>0.36289041628179808</v>
       </c>
       <c r="H26" s="3">
-        <v>4.6659198308134555e-003</v>
+        <v>3.5577491792333146e-003</v>
       </c>
       <c r="I26" s="3">
-        <v>-7.9283887468030723e-002</v>
+        <v>-5.943150684931503e-002</v>
       </c>
       <c r="J26" s="3">
-        <v>4.8327137546468446e-002</v>
+        <v>3.3755274261603407e-002</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="M26" s="2">
-        <v>19955500</v>
+        <v>187800</v>
       </c>
       <c r="N26" s="2">
-        <v>52865253.225806452</v>
+        <v>1118434.6456692913</v>
+      </c>
+      <c r="O26" s="3">
+        <v>-5.943150684931503e-002</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B27" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C27" s="2">
         <v>102</v>
       </c>
       <c r="D27" s="2">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E27" s="2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F27" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.86274509803921573</v>
       </c>
       <c r="G27" s="3">
-        <v>0.49698169701702288</v>
+        <v>0.50066403926478475</v>
       </c>
       <c r="H27" s="3">
-        <v>4.8723695785982636e-003</v>
+        <v>4.9084709731841642e-003</v>
       </c>
       <c r="I27" s="3">
-        <v>-8.333333333333337e-002</v>
+        <v>-7.4500000000000066e-002</v>
       </c>
       <c r="J27" s="3">
-        <v>4.4067796610169463e-002</v>
+        <v>5.9405940594059459e-002</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="M27" s="2">
-        <v>10025700</v>
+        <v>22579400</v>
       </c>
       <c r="N27" s="2">
-        <v>38547541.269841269</v>
+        <v>80933092.913385823</v>
+      </c>
+      <c r="O27" s="3">
+        <v>-7.4500000000000066e-002</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" s="2">
-        <v>126</v>
-      </c>
-      <c r="C28" s="2">
-        <v>102</v>
-      </c>
-      <c r="D28" s="2">
-        <v>85</v>
-      </c>
-      <c r="E28" s="2">
-        <v>17</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="G28" s="3">
-        <v>0.50181640446464071</v>
-      </c>
-      <c r="H28" s="3">
-        <v>4.9197686712219675e-003</v>
-      </c>
-      <c r="I28" s="3">
-        <v>-6.0312331717824463e-002</v>
-      </c>
-      <c r="J28" s="3">
-        <v>3.5322777101096214e-002</v>
-      </c>
-      <c r="K28" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="M28" s="2">
-        <v>219600</v>
-      </c>
-      <c r="N28" s="2">
-        <v>1077441.2698412698</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
     </row>
     <row r="29">
-      <c r="A29" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="2">
-        <v>124</v>
-      </c>
-      <c r="C29" s="2">
-        <v>100</v>
-      </c>
-      <c r="D29" s="2">
-        <v>83</v>
-      </c>
-      <c r="E29" s="2">
-        <v>17</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.82999999999999996</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.44164025485099134</v>
-      </c>
-      <c r="H29" s="3">
-        <v>4.4164025485099135e-003</v>
-      </c>
-      <c r="I29" s="3">
-        <v>-6.4490445859872625e-002</v>
-      </c>
-      <c r="J29" s="3">
-        <v>4.146730462519943e-002</v>
-      </c>
-      <c r="K29" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M29" s="2">
-        <v>710700</v>
-      </c>
-      <c r="N29" s="2">
-        <v>1562018.5483870967</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="2">
-        <v>124</v>
-      </c>
-      <c r="C30" s="2">
-        <v>100</v>
-      </c>
-      <c r="D30" s="2">
-        <v>83</v>
-      </c>
-      <c r="E30" s="2">
-        <v>17</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.82999999999999996</v>
-      </c>
-      <c r="G30" s="3">
-        <v>0.48704419530700516</v>
-      </c>
-      <c r="H30" s="3">
-        <v>4.8704419530700514e-003</v>
-      </c>
-      <c r="I30" s="3">
-        <v>-4.7619047619047672e-002</v>
-      </c>
-      <c r="J30" s="3">
-        <v>2.1195274496177863e-002</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M30" s="2">
-        <v>28713600</v>
-      </c>
-      <c r="N30" s="2">
-        <v>72691002.419354841</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="2">
-        <v>126</v>
-      </c>
-      <c r="C31" s="2">
-        <v>102</v>
-      </c>
-      <c r="D31" s="2">
-        <v>84</v>
-      </c>
-      <c r="E31" s="2">
-        <v>18</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="G31" s="3">
-        <v>0.39103372364312827</v>
-      </c>
-      <c r="H31" s="3">
-        <v>3.8336639572855713e-003</v>
-      </c>
-      <c r="I31" s="3">
-        <v>-7.251317012705305e-002</v>
-      </c>
-      <c r="J31" s="3">
-        <v>4.3463263194204904e-002</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="M31" s="2">
-        <v>6224000</v>
-      </c>
-      <c r="N31" s="2">
-        <v>18288660.714285713</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" s="2">
-        <v>126</v>
-      </c>
-      <c r="C32" s="2">
-        <v>102</v>
-      </c>
-      <c r="D32" s="2">
-        <v>84</v>
-      </c>
-      <c r="E32" s="2">
-        <v>18</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.82352941176470584</v>
-      </c>
-      <c r="G32" s="3">
-        <v>0.37001306745879115</v>
-      </c>
-      <c r="H32" s="3">
-        <v>3.6275790927332466e-003</v>
-      </c>
-      <c r="I32" s="3">
-        <v>-0.12493074792243775</v>
-      </c>
-      <c r="J32" s="3">
-        <v>4.4634377967711414e-002</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M32" s="2">
-        <v>760400</v>
-      </c>
-      <c r="N32" s="2">
-        <v>4218193.6507936511</v>
-      </c>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
     </row>
     <row r="33">
-      <c r="A33" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B33" s="2">
-        <v>124</v>
-      </c>
-      <c r="C33" s="2">
-        <v>100</v>
-      </c>
-      <c r="D33" s="2">
-        <v>82</v>
-      </c>
-      <c r="E33" s="2">
-        <v>18</v>
-      </c>
-      <c r="F33" s="3">
-        <v>0.81999999999999995</v>
-      </c>
-      <c r="G33" s="3">
-        <v>0.42889426198251868</v>
-      </c>
-      <c r="H33" s="3">
-        <v>4.2889426198251864e-003</v>
-      </c>
-      <c r="I33" s="3">
-        <v>-8.8235294117646967e-002</v>
-      </c>
-      <c r="J33" s="3">
-        <v>6.800000000000006e-002</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="M33" s="2">
-        <v>10743200</v>
-      </c>
-      <c r="N33" s="2">
-        <v>32943161.290322579</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34" s="2">
-        <v>124</v>
-      </c>
-      <c r="C34" s="2">
-        <v>100</v>
-      </c>
-      <c r="D34" s="2">
-        <v>82</v>
-      </c>
-      <c r="E34" s="2">
-        <v>18</v>
-      </c>
-      <c r="F34" s="3">
-        <v>0.81999999999999995</v>
-      </c>
-      <c r="G34" s="3">
-        <v>0.34704850463548864</v>
-      </c>
-      <c r="H34" s="3">
-        <v>3.4704850463548862e-003</v>
-      </c>
-      <c r="I34" s="3">
-        <v>-4.0569395017793664e-002</v>
-      </c>
-      <c r="J34" s="3">
-        <v>5.4072096128170877e-002</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M34" s="2">
-        <v>2250700</v>
-      </c>
-      <c r="N34" s="2">
-        <v>6623943.5483870972</v>
-      </c>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
     </row>
     <row r="35">
-      <c r="A35" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B35" s="2">
-        <v>122</v>
-      </c>
-      <c r="C35" s="2">
-        <v>99</v>
-      </c>
-      <c r="D35" s="2">
-        <v>81</v>
-      </c>
-      <c r="E35" s="2">
-        <v>18</v>
-      </c>
-      <c r="F35" s="3">
-        <v>0.81818181818181823</v>
-      </c>
-      <c r="G35" s="3">
-        <v>0.30065437361679193</v>
-      </c>
-      <c r="H35" s="3">
-        <v>3.03691286481608e-003</v>
-      </c>
-      <c r="I35" s="3">
-        <v>-8.969907407407407e-002</v>
-      </c>
-      <c r="J35" s="3">
-        <v>4.0634291377601661e-002</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="M35" s="2">
-        <v>4754300</v>
-      </c>
-      <c r="N35" s="2">
-        <v>11394263.934426229</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B36" s="2">
-        <v>124</v>
-      </c>
-      <c r="C36" s="2">
-        <v>100</v>
-      </c>
-      <c r="D36" s="2">
-        <v>81</v>
-      </c>
-      <c r="E36" s="2">
-        <v>19</v>
-      </c>
-      <c r="F36" s="3">
-        <v>0.81000000000000005</v>
-      </c>
-      <c r="G36" s="3">
-        <v>0.43913719655277089</v>
-      </c>
-      <c r="H36" s="3">
-        <v>4.3913719655277088e-003</v>
-      </c>
-      <c r="I36" s="3">
-        <v>-6.5882352941176392e-002</v>
-      </c>
-      <c r="J36" s="3">
-        <v>3.47947112038971e-002</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M36" s="2">
-        <v>741300</v>
-      </c>
-      <c r="N36" s="2">
-        <v>3545499.1935483869</v>
-      </c>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="2">
-        <v>126</v>
-      </c>
-      <c r="C37" s="2">
-        <v>102</v>
-      </c>
-      <c r="D37" s="2">
-        <v>82</v>
-      </c>
-      <c r="E37" s="2">
-        <v>20</v>
-      </c>
-      <c r="F37" s="3">
-        <v>0.80392156862745101</v>
-      </c>
-      <c r="G37" s="3">
-        <v>0.65584748529982806</v>
-      </c>
-      <c r="H37" s="3">
-        <v>6.4298773068610596e-003</v>
-      </c>
-      <c r="I37" s="3">
-        <v>-6.4788732394366222e-002</v>
-      </c>
-      <c r="J37" s="3">
-        <v>0.21229050279329598</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="M37" s="2">
-        <v>263400</v>
-      </c>
-      <c r="N37" s="2">
-        <v>990836.50793650793</v>
-      </c>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="2">
-        <v>124</v>
-      </c>
-      <c r="C38" s="2">
-        <v>100</v>
-      </c>
-      <c r="D38" s="2">
-        <v>79</v>
-      </c>
-      <c r="E38" s="2">
-        <v>21</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0.79000000000000004</v>
-      </c>
-      <c r="G38" s="3">
-        <v>0.33581892811874259</v>
-      </c>
-      <c r="H38" s="3">
-        <v>3.3581892811874259e-003</v>
-      </c>
-      <c r="I38" s="3">
-        <v>-3.5683202785030455e-002</v>
-      </c>
-      <c r="J38" s="3">
-        <v>1.870078740157477e-002</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="M38" s="2">
-        <v>191100</v>
-      </c>
-      <c r="N38" s="2">
-        <v>491350</v>
-      </c>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="2">
-        <v>122</v>
-      </c>
-      <c r="C39" s="2">
-        <v>99</v>
-      </c>
-      <c r="D39" s="2">
-        <v>78</v>
-      </c>
-      <c r="E39" s="2">
-        <v>21</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0.78787878787878785</v>
-      </c>
-      <c r="G39" s="3">
-        <v>0.33005272270238717</v>
-      </c>
-      <c r="H39" s="3">
-        <v>3.3338658858826989e-003</v>
-      </c>
-      <c r="I39" s="3">
-        <v>-5.729596042868923e-002</v>
-      </c>
-      <c r="J39" s="3">
-        <v>3.3110119047619069e-002</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="M39" s="2">
-        <v>4096300</v>
-      </c>
-      <c r="N39" s="2">
-        <v>12714905.737704918</v>
-      </c>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="2">
-        <v>126</v>
-      </c>
-      <c r="C40" s="2">
-        <v>102</v>
-      </c>
-      <c r="D40" s="2">
-        <v>80</v>
-      </c>
-      <c r="E40" s="2">
-        <v>22</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0.78431372549019607</v>
-      </c>
-      <c r="G40" s="3">
-        <v>0.32350989053499685</v>
-      </c>
-      <c r="H40" s="3">
-        <v>3.1716655934803614e-003</v>
-      </c>
-      <c r="I40" s="3">
-        <v>-5.1502145922746823e-002</v>
-      </c>
-      <c r="J40" s="3">
-        <v>2.6373626373626502e-002</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="M40" s="2">
-        <v>364700</v>
-      </c>
-      <c r="N40" s="2">
-        <v>1041146.0317460317</v>
-      </c>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B41" s="2">
-        <v>126</v>
-      </c>
-      <c r="C41" s="2">
-        <v>102</v>
-      </c>
-      <c r="D41" s="2">
-        <v>80</v>
-      </c>
-      <c r="E41" s="2">
-        <v>22</v>
-      </c>
-      <c r="F41" s="3">
-        <v>0.78431372549019607</v>
-      </c>
-      <c r="G41" s="3">
-        <v>0.36297802941709412</v>
-      </c>
-      <c r="H41" s="3">
-        <v>3.5586081315401386e-003</v>
-      </c>
-      <c r="I41" s="3">
-        <v>-5.0974512743628186e-002</v>
-      </c>
-      <c r="J41" s="3">
-        <v>7.986111111111116e-002</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" s="2">
-        <v>242800</v>
-      </c>
-      <c r="N41" s="2">
-        <v>1169809.5238095238</v>
-      </c>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B42" s="2">
-        <v>124</v>
-      </c>
-      <c r="C42" s="2">
-        <v>100</v>
-      </c>
-      <c r="D42" s="2">
-        <v>78</v>
-      </c>
-      <c r="E42" s="2">
-        <v>22</v>
-      </c>
-      <c r="F42" s="3">
-        <v>0.78000000000000003</v>
-      </c>
-      <c r="G42" s="3">
-        <v>0.37405978775583049</v>
-      </c>
-      <c r="H42" s="3">
-        <v>3.7405978775583047e-003</v>
-      </c>
-      <c r="I42" s="3">
-        <v>-5.0558807876529999e-002</v>
-      </c>
-      <c r="J42" s="3">
-        <v>4.6145913895333734e-002</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="M42" s="2">
-        <v>1420000</v>
-      </c>
-      <c r="N42" s="2">
-        <v>3940632.2580645164</v>
-      </c>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
     </row>
     <row r="43">
-      <c r="A43" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B43" s="2">
-        <v>124</v>
-      </c>
-      <c r="C43" s="2">
-        <v>100</v>
-      </c>
-      <c r="D43" s="2">
-        <v>78</v>
-      </c>
-      <c r="E43" s="2">
-        <v>22</v>
-      </c>
-      <c r="F43" s="3">
-        <v>0.78000000000000003</v>
-      </c>
-      <c r="G43" s="3">
-        <v>0.31765567648855336</v>
-      </c>
-      <c r="H43" s="3">
-        <v>3.1765567648855335e-003</v>
-      </c>
-      <c r="I43" s="3">
-        <v>-3.7709497206704023e-002</v>
-      </c>
-      <c r="J43" s="3">
-        <v>5.4961832061068749e-002</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="M43" s="2">
-        <v>293200</v>
-      </c>
-      <c r="N43" s="2">
-        <v>1286870.1612903227</v>
-      </c>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44">
-      <c r="A44" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="2">
-        <v>124</v>
-      </c>
-      <c r="C44" s="2">
-        <v>100</v>
-      </c>
-      <c r="D44" s="2">
-        <v>78</v>
-      </c>
-      <c r="E44" s="2">
-        <v>22</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.78000000000000003</v>
-      </c>
-      <c r="G44" s="3">
-        <v>0.34376321515077685</v>
-      </c>
-      <c r="H44" s="3">
-        <v>3.4376321515077685e-003</v>
-      </c>
-      <c r="I44" s="3">
-        <v>-3.9622641509433953e-002</v>
-      </c>
-      <c r="J44" s="3">
-        <v>2.6897214217098897e-002</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M44" s="2">
-        <v>763200</v>
-      </c>
-      <c r="N44" s="2">
-        <v>2641660.4838709678</v>
-      </c>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="2">
-        <v>126</v>
-      </c>
-      <c r="C45" s="2">
-        <v>102</v>
-      </c>
-      <c r="D45" s="2">
-        <v>79</v>
-      </c>
-      <c r="E45" s="2">
-        <v>23</v>
-      </c>
-      <c r="F45" s="3">
-        <v>0.77450980392156865</v>
-      </c>
-      <c r="G45" s="3">
-        <v>0.384153819966701</v>
-      </c>
-      <c r="H45" s="3">
-        <v>3.7662139212421668e-003</v>
-      </c>
-      <c r="I45" s="3">
-        <v>-3.8922155688622673e-002</v>
-      </c>
-      <c r="J45" s="3">
-        <v>2.6119402985074647e-002</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="M45" s="2">
-        <v>298500</v>
-      </c>
-      <c r="N45" s="2">
-        <v>824760.31746031751</v>
-      </c>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B46" s="2">
-        <v>126</v>
-      </c>
-      <c r="C46" s="2">
-        <v>102</v>
-      </c>
-      <c r="D46" s="2">
-        <v>78</v>
-      </c>
-      <c r="E46" s="2">
-        <v>24</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.76470588235294112</v>
-      </c>
-      <c r="G46" s="3">
-        <v>0.31579964575155228</v>
-      </c>
-      <c r="H46" s="3">
-        <v>3.0960749583485519e-003</v>
-      </c>
-      <c r="I46" s="3">
-        <v>-5.6634304207119679e-002</v>
-      </c>
-      <c r="J46" s="3">
-        <v>3.7300177619893349e-002</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="M46" s="2">
-        <v>129600</v>
-      </c>
-      <c r="N46" s="2">
-        <v>489063.49206349207</v>
-      </c>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B47" s="2">
-        <v>124</v>
-      </c>
-      <c r="C47" s="2">
-        <v>100</v>
-      </c>
-      <c r="D47" s="2">
-        <v>76</v>
-      </c>
-      <c r="E47" s="2">
-        <v>24</v>
-      </c>
-      <c r="F47" s="3">
-        <v>0.76000000000000001</v>
-      </c>
-      <c r="G47" s="3">
-        <v>0.31294959268031647</v>
-      </c>
-      <c r="H47" s="3">
-        <v>3.1294959268031645e-003</v>
-      </c>
-      <c r="I47" s="3">
-        <v>-4.4004400440044056e-002</v>
-      </c>
-      <c r="J47" s="3">
-        <v>6.321839080459779e-002</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="M47" s="2">
-        <v>5703700</v>
-      </c>
-      <c r="N47" s="2">
-        <v>18409722.580645163</v>
-      </c>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="2">
-        <v>124</v>
-      </c>
-      <c r="C48" s="2">
-        <v>100</v>
-      </c>
-      <c r="D48" s="2">
-        <v>76</v>
-      </c>
-      <c r="E48" s="2">
-        <v>24</v>
-      </c>
-      <c r="F48" s="3">
-        <v>0.76000000000000001</v>
-      </c>
-      <c r="G48" s="3">
-        <v>0.51379454890483622</v>
-      </c>
-      <c r="H48" s="3">
-        <v>5.1379454890483622e-003</v>
-      </c>
-      <c r="I48" s="3">
-        <v>-0.20000000000000007</v>
-      </c>
-      <c r="J48" s="3">
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="M48" s="2">
-        <v>243700</v>
-      </c>
-      <c r="N48" s="2">
-        <v>1202063.7096774194</v>
-      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
     </row>
     <row r="49">
       <c r="F49" s="6"/>
@@ -4333,16 +3646,10 @@
       <c r="I213" s="6"/>
       <c r="J213" s="6"/>
     </row>
-    <row r="214">
-      <c r="F214" s="6"/>
-      <c r="G214" s="6"/>
-      <c r="H214" s="6"/>
-      <c r="I214" s="6"/>
-      <c r="J214" s="6"/>
-    </row>
+    <row r="214"/>
   </sheetData>
-  <sortState ref="A2:N214" columnSort="0">
-    <sortCondition sortBy="value" descending="0" ref="I2:I214"/>
+  <sortState ref="A1:N47" columnSort="0">
+    <sortCondition sortBy="value" descending="0" ref="I1:I47"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="P2:Z11"/>

</xml_diff>